<commit_message>
Added dockerized selenium grid layer
</commit_message>
<xml_diff>
--- a/target/test-classes/excel/Batch.xlsx
+++ b/target/test-classes/excel/Batch.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksh\git\Selenium-Java-DataDriven-AFW\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksh\git\selenium-AFW\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E1F2E7-6405-4902-BC2C-2C36505C7CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC9F41D-EEF2-4879-B43D-B91B6303ED9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>TestName</t>
   </si>
@@ -50,19 +50,19 @@
     <t>No</t>
   </si>
   <si>
-    <t>login_validation</t>
-  </si>
-  <si>
-    <t>login_validation_copy</t>
-  </si>
-  <si>
     <t>InvocationCount</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>TestDescription</t>
+  </si>
+  <si>
+    <t>This is a test to validate login in to OrangeHrm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a copy </t>
+  </si>
+  <si>
+    <t>login</t>
   </si>
 </sst>
 </file>
@@ -100,7 +100,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,51 +381,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
+      <c r="D3" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>